<commit_message>
Adding repetitive inv mass fit
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>V2</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Rel Error</t>
+  </si>
+  <si>
+    <t>8 TeV</t>
   </si>
 </sst>
 </file>
@@ -106,8 +109,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -126,14 +145,14 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -141,6 +160,14 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -148,6 +175,14 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -570,7 +605,7 @@
       <c r="B6" s="1">
         <v>8.2700000000000004E-4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1.2711899999999999E-5</v>
       </c>
       <c r="F6" s="1">
@@ -593,7 +628,7 @@
       <c r="B7" s="1">
         <v>6.2500000000000001E-4</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3"/>
       <c r="F7" s="1">
         <f>B7^2/C2 + C6^2*0.25*B3^2/(C2)^3</f>
         <v>3.3106023250577236E-5</v>
@@ -611,9 +646,138 @@
         <v>5.7537833857886269E-3</v>
       </c>
     </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0265E-2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5.0289999999999996E-3</v>
+      </c>
+      <c r="D16">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="F16" s="1">
+        <f>B16/SQRT(C16)</f>
+        <v>0.14474985451386693</v>
+      </c>
+      <c r="H16">
+        <f>(F16-(1-D16)*F17)/(D16)</f>
+        <v>0.14476620966294818</v>
+      </c>
+      <c r="K16">
+        <f>J20/H16</f>
+        <v>1.7326847084940263E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.02398E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>B17/SQRT(C16)</f>
+        <v>0.14439450172928345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.69605E-4</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5.9501299999999996E-7</v>
+      </c>
+      <c r="F20" s="1">
+        <f>B20^2/C16 + C20^2*0.25*B16^2/(C16)^3</f>
+        <v>5.720068559988449E-6</v>
+      </c>
+      <c r="H20">
+        <f>F20/(D16)^2 + F21*((1-D16)/D16)^2</f>
+        <v>6.2917794780767462E-6</v>
+      </c>
+      <c r="J20">
+        <f>SQRT(H20)</f>
+        <v>2.5083419778963046E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.8015599999999999E-4</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="F21" s="1">
+        <f>B21^2/C16 + C20^2*0.25*B17^2/(C16)^3</f>
+        <v>1.5607029487138288E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="F23">
+        <f>SQRT(F20)</f>
+        <v>2.391666481762967E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="F24">
+        <f>SQRT(F21)</f>
+        <v>3.9505733111965266E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Commit prior to start of work
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="27">
   <si>
     <t>V2</t>
   </si>
@@ -62,12 +62,54 @@
   <si>
     <t>8 TeV</t>
   </si>
+  <si>
+    <t>NO PT CUT</t>
+  </si>
+  <si>
+    <t>PT CUT</t>
+  </si>
+  <si>
+    <t>1-1.4</t>
+  </si>
+  <si>
+    <t>1.4-1.8</t>
+  </si>
+  <si>
+    <t>1.8-2.2</t>
+  </si>
+  <si>
+    <t>2.2-2.8</t>
+  </si>
+  <si>
+    <t>2.8-3.6</t>
+  </si>
+  <si>
+    <t>3.6-4.6</t>
+  </si>
+  <si>
+    <t>Pt Bins</t>
+  </si>
+  <si>
+    <t>4.6-6</t>
+  </si>
+  <si>
+    <t>v2 signal</t>
+  </si>
+  <si>
+    <t>Relative Error</t>
+  </si>
+  <si>
+    <t>PT CUT (Almost all of PD1-4)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,13 +133,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,7 +164,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,18 +196,89 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -168,6 +294,31 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -183,6 +334,31 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,15 +688,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:AB109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="L88" workbookViewId="0">
+      <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -605,7 +783,7 @@
       <c r="B6" s="1">
         <v>8.2700000000000004E-4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="9">
         <v>1.2711899999999999E-5</v>
       </c>
       <c r="F6" s="1">
@@ -628,7 +806,7 @@
       <c r="B7" s="1">
         <v>6.2500000000000001E-4</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="10"/>
       <c r="F7" s="1">
         <f>B7^2/C2 + C6^2*0.25*B3^2/(C2)^3</f>
         <v>3.3106023250577236E-5</v>
@@ -651,6 +829,21 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+    </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>0</v>
@@ -700,7 +893,7 @@
         <v>1.7326847084940263E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -712,7 +905,7 @@
         <v>0.14439450172928345</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -726,14 +919,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1">
         <v>1.69605E-4</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="9">
         <v>5.9501299999999996E-7</v>
       </c>
       <c r="F20" s="1">
@@ -749,35 +942,2275 @@
         <v>2.5083419778963046E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="1">
         <v>2.8015599999999999E-4</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="10"/>
       <c r="F21" s="1">
         <f>B21^2/C16 + C20^2*0.25*B17^2/(C16)^3</f>
         <v>1.5607029487138288E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:28">
       <c r="F23">
         <f>SQRT(F20)</f>
         <v>2.391666481762967E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:28">
       <c r="F24">
         <f>SQRT(F21)</f>
         <v>3.9505733111965266E-3</v>
       </c>
     </row>
+    <row r="26" spans="1:28">
+      <c r="A26" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="R26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+    </row>
+    <row r="27" spans="1:28">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="R27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" t="s">
+        <v>0</v>
+      </c>
+      <c r="S28" t="s">
+        <v>3</v>
+      </c>
+      <c r="T28" t="s">
+        <v>4</v>
+      </c>
+      <c r="U28" t="s">
+        <v>6</v>
+      </c>
+      <c r="W28" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3.9086800000000003E-3</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="D29">
+        <v>0.95326699999999998</v>
+      </c>
+      <c r="F29" s="1">
+        <f>B29/SQRT(C29)</f>
+        <v>5.5114294993109846E-2</v>
+      </c>
+      <c r="H29" s="4">
+        <f>(F29-(1-D29)*F30)/(D29)</f>
+        <v>5.6368121446440135E-2</v>
+      </c>
+      <c r="K29">
+        <f>J33/H29</f>
+        <v>0.30290081543083358</v>
+      </c>
+      <c r="N29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" s="6">
+        <v>5.63681214464401E-2</v>
+      </c>
+      <c r="P29" s="5">
+        <v>0.30290081543083358</v>
+      </c>
+      <c r="R29" t="s">
+        <v>1</v>
+      </c>
+      <c r="S29" s="1">
+        <v>3.5723600000000001E-3</v>
+      </c>
+      <c r="T29" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="U29">
+        <v>0.95326699999999998</v>
+      </c>
+      <c r="W29" s="1">
+        <f>S29/SQRT(T29)</f>
+        <v>5.0372018907044291E-2</v>
+      </c>
+      <c r="Y29" s="4">
+        <f>(W29-(1-U29)*W30)/(U29)</f>
+        <v>5.1750072214157193E-2</v>
+      </c>
+      <c r="AB29">
+        <f>AA33/Y29</f>
+        <v>0.29685578521723788</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2.09486E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f>B30/SQRT(C29)</f>
+        <v>2.9538548054398438E-2</v>
+      </c>
+      <c r="N30" t="s">
+        <v>17</v>
+      </c>
+      <c r="O30" s="7">
+        <v>6.4875933775467298E-2</v>
+      </c>
+      <c r="P30" s="5">
+        <v>0.131491250810882</v>
+      </c>
+      <c r="R30" t="s">
+        <v>2</v>
+      </c>
+      <c r="S30" s="1">
+        <v>1.57883E-3</v>
+      </c>
+      <c r="W30" s="1">
+        <f>S30/SQRT(T29)</f>
+        <v>2.226227329020836E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28">
+      <c r="N31" t="s">
+        <v>18</v>
+      </c>
+      <c r="O31" s="7">
+        <v>0.1099989609524949</v>
+      </c>
+      <c r="P31" s="5">
+        <v>6.5087491546706247E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N32" t="s">
+        <v>19</v>
+      </c>
+      <c r="O32" s="7">
+        <v>0.12630714105509813</v>
+      </c>
+      <c r="P32" s="5">
+        <v>4.0820441896712134E-2</v>
+      </c>
+      <c r="R32" t="s">
+        <v>8</v>
+      </c>
+      <c r="W32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.1517999999999999E-3</v>
+      </c>
+      <c r="C33" s="9">
+        <v>5.9501299999999996E-7</v>
+      </c>
+      <c r="F33" s="1">
+        <f>B33^2/C29 + C33^2*0.25*B29^2/(C29)^3</f>
+        <v>2.6376820598442998E-4</v>
+      </c>
+      <c r="H33">
+        <f>F33/(D29)^2 + F34*((1-D29)/D29)^2</f>
+        <v>2.915197669098219E-4</v>
+      </c>
+      <c r="J33">
+        <f>SQRT(H33)</f>
+        <v>1.7073949950430975E-2</v>
+      </c>
+      <c r="N33" t="s">
+        <v>20</v>
+      </c>
+      <c r="O33" s="7">
+        <v>0.15316548557983833</v>
+      </c>
+      <c r="P33" s="5">
+        <v>3.1950323854232042E-2</v>
+      </c>
+      <c r="R33" t="s">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1.03633E-3</v>
+      </c>
+      <c r="T33" s="13">
+        <v>5.3852999999999999E-7</v>
+      </c>
+      <c r="W33" s="1">
+        <f>S33^2/T29 + T33^2*0.25*S29^2/(T29)^3</f>
+        <v>2.1353272151489641E-4</v>
+      </c>
+      <c r="Y33">
+        <f>W33/(U29)^2 + W34*((1-U29)/U29)^2</f>
+        <v>2.3600051698579458E-4</v>
+      </c>
+      <c r="AA33">
+        <f>SQRT(Y33)</f>
+        <v>1.5362308322182399E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.62104E-3</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="F34" s="1">
+        <f>B34^2/C29 + C33^2*0.25*B30^2/(C29)^3</f>
+        <v>5.2246324682272364E-4</v>
+      </c>
+      <c r="N34" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="7">
+        <v>0.1822977368690569</v>
+      </c>
+      <c r="P34" s="5">
+        <v>3.3873671896799913E-2</v>
+      </c>
+      <c r="R34" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" s="1">
+        <v>1.4596800000000001E-3</v>
+      </c>
+      <c r="T34" s="14"/>
+      <c r="W34" s="1">
+        <f>S34^2/T29 + T33^2*0.25*S30^2/(T29)^3</f>
+        <v>4.2362696478521518E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28">
+      <c r="N35" t="s">
+        <v>23</v>
+      </c>
+      <c r="O35" s="7">
+        <v>0.21770241685354796</v>
+      </c>
+      <c r="P35" s="5">
+        <v>4.7980277714905512E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
+      <c r="F36">
+        <f>SQRT(F33)</f>
+        <v>1.6240942275140009E-2</v>
+      </c>
+      <c r="W36">
+        <f>SQRT(W33)</f>
+        <v>1.4612758860492306E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
+      <c r="F37">
+        <f>SQRT(F34)</f>
+        <v>2.285745495068783E-2</v>
+      </c>
+      <c r="W37">
+        <f>SQRT(W34)</f>
+        <v>2.0582200193011806E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="R39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
+      <c r="A40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" t="s">
+        <v>12</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V40" s="2"/>
+      <c r="W40" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
+      <c r="A41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="3">
+        <v>4.66936E-3</v>
+      </c>
+      <c r="C41" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.953677</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="1">
+        <f>B41/SQRT(C41)</f>
+        <v>6.5840254118788785E-2</v>
+      </c>
+      <c r="H41">
+        <f>(F41-(1-D41)*F42)/(D41)</f>
+        <v>6.4878642483089902E-2</v>
+      </c>
+      <c r="K41">
+        <f>J45/H41</f>
+        <v>0.13149125081340679</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S41" s="3">
+        <v>5.0995099999999998E-3</v>
+      </c>
+      <c r="T41" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="U41" s="2">
+        <v>0.953677</v>
+      </c>
+      <c r="V41" s="2"/>
+      <c r="W41" s="1">
+        <f>S41/SQRT(T41)</f>
+        <v>7.1905578983266355E-2</v>
+      </c>
+      <c r="Y41">
+        <f>(W41-(1-U41)*W42)/(U41)</f>
+        <v>7.1787446794090104E-2</v>
+      </c>
+      <c r="AB41">
+        <f>AA45/Y41</f>
+        <v>0.10656287981727336</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
+      <c r="A42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="3">
+        <v>6.0733699999999998E-3</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="1">
+        <f>B42/SQRT(C41)</f>
+        <v>8.5637480116638742E-2</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S42" s="3">
+        <v>5.2719899999999998E-3</v>
+      </c>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="1">
+        <f>S42/SQRT(T41)</f>
+        <v>7.4337631133969823E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+    </row>
+    <row r="44" spans="1:28">
+      <c r="A44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" t="s">
+        <v>10</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
+      <c r="A45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="3">
+        <v>5.7454399999999997E-4</v>
+      </c>
+      <c r="C45" s="8">
+        <v>5.9500000000000002E-7</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="1">
+        <f>B45^2/C41 + C45^2*0.25*B41^2/(C41)^3</f>
+        <v>6.5631898531995209E-5</v>
+      </c>
+      <c r="H45">
+        <f>F45/(D41)^2 + F46*((1-D41)/D41)^2</f>
+        <v>7.2777514849471254E-5</v>
+      </c>
+      <c r="J45">
+        <f>SQRT(H45)</f>
+        <v>8.5309738511773238E-3</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S45" s="3">
+        <v>5.1518099999999997E-4</v>
+      </c>
+      <c r="T45" s="12">
+        <v>5.3852999999999999E-7</v>
+      </c>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="1">
+        <f>S45^2/T41 + T45^2*0.25*S41^2/(T41)^3</f>
+        <v>5.2770119432398038E-5</v>
+      </c>
+      <c r="Y45">
+        <f>W45/(U41)^2 + W46*((1-U41)/U41)^2</f>
+        <v>5.8520619111258179E-5</v>
+      </c>
+      <c r="AA45">
+        <f>SQRT(Y45)</f>
+        <v>7.649877065107529E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
+      <c r="A46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1.1448999999999999E-3</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="1">
+        <f>B46^2/C41 + C45^2*0.25*B42^2/(C41)^3</f>
+        <v>2.6061741518249173E-4</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S46" s="3">
+        <v>1.03199E-3</v>
+      </c>
+      <c r="T46" s="12"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="1">
+        <f>S46^2/T41 + T45^2*0.25*S42^2/(T41)^3</f>
+        <v>2.1174798686191657E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+    </row>
+    <row r="48" spans="1:28">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48">
+        <f>SQRT(F45)</f>
+        <v>8.1013516484593606E-3</v>
+      </c>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48">
+        <f>SQRT(W45)</f>
+        <v>7.2643044699680671E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49">
+        <f>SQRT(F46)</f>
+        <v>1.6143649376225058E-2</v>
+      </c>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49">
+        <f>SQRT(W46)</f>
+        <v>1.4551563038447676E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="R51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28">
+      <c r="A52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" t="s">
+        <v>7</v>
+      </c>
+      <c r="K52" t="s">
+        <v>12</v>
+      </c>
+      <c r="R52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V52" s="2"/>
+      <c r="W52" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28">
+      <c r="A53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="3">
+        <v>7.8558699999999992E-3</v>
+      </c>
+      <c r="C53" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.95487200000000005</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="1">
+        <f>B53/SQRT(C53)</f>
+        <v>0.1107715997747377</v>
+      </c>
+      <c r="H53">
+        <f>(F53-(1-D53)*F54)/(D53)</f>
+        <v>0.11000355364205899</v>
+      </c>
+      <c r="K53">
+        <f>J57/H53</f>
+        <v>6.5087491551711077E-2</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S53" s="3">
+        <v>7.6369599999999999E-3</v>
+      </c>
+      <c r="T53" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="U53" s="2">
+        <v>0.95487200000000005</v>
+      </c>
+      <c r="V53" s="2"/>
+      <c r="W53" s="1">
+        <f>S53/SQRT(T53)</f>
+        <v>0.10768486197145331</v>
+      </c>
+      <c r="Y53">
+        <f>(W53-(1-U53)*W54)/(U53)</f>
+        <v>0.10711039174623081</v>
+      </c>
+      <c r="AB53">
+        <f>AA57/Y53</f>
+        <v>5.9928084209284999E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28">
+      <c r="A54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="3">
+        <v>9.0083999999999997E-3</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="1">
+        <f>B54/SQRT(C53)</f>
+        <v>0.12702283507883241</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S54" s="3">
+        <v>8.4990099999999996E-3</v>
+      </c>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="1">
+        <f>S54/SQRT(T53)</f>
+        <v>0.11984018755421023</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+    </row>
+    <row r="56" spans="1:28">
+      <c r="A56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" t="s">
+        <v>10</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28">
+      <c r="A57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="3">
+        <v>4.8321799999999999E-4</v>
+      </c>
+      <c r="C57" s="8">
+        <v>5.9500000000000002E-7</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="1">
+        <f>B57^2/C53 + C57^2*0.25*B53^2/(C53)^3</f>
+        <v>4.6425318107492967E-5</v>
+      </c>
+      <c r="H57">
+        <f>F57/(D53)^2 + F58*((1-D53)/D53)^2</f>
+        <v>5.126352889548571E-5</v>
+      </c>
+      <c r="J57">
+        <f>SQRT(H57)</f>
+        <v>7.1598553683357114E-3</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S57" s="3">
+        <v>4.3320199999999999E-4</v>
+      </c>
+      <c r="T57" s="12">
+        <v>5.3852999999999999E-7</v>
+      </c>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="1">
+        <f>S57^2/T53 + T57^2*0.25*S53^2/(T53)^3</f>
+        <v>3.7312089670696186E-5</v>
+      </c>
+      <c r="Y57">
+        <f>W57/(U53)^2 + W58*((1-U53)/U53)^2</f>
+        <v>4.120254136430352E-5</v>
+      </c>
+      <c r="AA57">
+        <f>SQRT(Y57)</f>
+        <v>6.4189205762576248E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28">
+      <c r="A58" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="3">
+        <v>8.8309E-4</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="1">
+        <f>B58^2/C53 + C57^2*0.25*B54^2/(C53)^3</f>
+        <v>1.5505235666326631E-4</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S58" s="3">
+        <v>7.94489E-4</v>
+      </c>
+      <c r="T58" s="12"/>
+      <c r="U58" s="2"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="1">
+        <f>S58^2/T53 + T57^2*0.25*S54^2/(T53)^3</f>
+        <v>1.2550013682074651E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="R59" s="2"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
+      <c r="U59" s="2"/>
+      <c r="V59" s="2"/>
+    </row>
+    <row r="60" spans="1:28">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60">
+        <f>SQRT(F57)</f>
+        <v>6.8136127060094169E-3</v>
+      </c>
+      <c r="R60" s="2"/>
+      <c r="S60" s="2"/>
+      <c r="T60" s="2"/>
+      <c r="U60" s="2"/>
+      <c r="V60" s="2"/>
+      <c r="W60">
+        <f>SQRT(W57)</f>
+        <v>6.1083622740220793E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61">
+        <f>SQRT(F58)</f>
+        <v>1.2452002114650732E-2</v>
+      </c>
+      <c r="R61" s="2"/>
+      <c r="S61" s="2"/>
+      <c r="T61" s="2"/>
+      <c r="U61" s="2"/>
+      <c r="V61" s="2"/>
+      <c r="W61">
+        <f>SQRT(W58)</f>
+        <v>1.1202684357811145E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="R63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28">
+      <c r="A64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" t="s">
+        <v>5</v>
+      </c>
+      <c r="H64" t="s">
+        <v>7</v>
+      </c>
+      <c r="K64" t="s">
+        <v>12</v>
+      </c>
+      <c r="R64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V64" s="2"/>
+      <c r="W64" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28">
+      <c r="A65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="3">
+        <v>9.0376399999999996E-3</v>
+      </c>
+      <c r="C65" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.95613999999999999</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="1">
+        <f>B65/SQRT(C65)</f>
+        <v>0.12743513334464043</v>
+      </c>
+      <c r="H65">
+        <f>(F65-(1-D65)*F66)/(D65)</f>
+        <v>0.12631241464571724</v>
+      </c>
+      <c r="K65">
+        <f>J69/H65</f>
+        <v>4.0820441904701729E-2</v>
+      </c>
+      <c r="R65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S65" s="3">
+        <v>9.0660500000000008E-3</v>
+      </c>
+      <c r="T65" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="U65" s="2">
+        <v>0.95613999999999999</v>
+      </c>
+      <c r="V65" s="2"/>
+      <c r="W65" s="1">
+        <f>S65/SQRT(T65)</f>
+        <v>0.12783572820550251</v>
+      </c>
+      <c r="Y65">
+        <f>(W65-(1-U65)*W66)/(U65)</f>
+        <v>0.12682808468040832</v>
+      </c>
+      <c r="AB65">
+        <f>AA69/Y65</f>
+        <v>3.6521420558687623E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28">
+      <c r="A66" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="3">
+        <v>1.0773400000000001E-2</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="1">
+        <f>B66/SQRT(C65)</f>
+        <v>0.15191019619891361</v>
+      </c>
+      <c r="R66" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S66" s="3">
+        <v>1.06239E-2</v>
+      </c>
+      <c r="T66" s="2"/>
+      <c r="U66" s="2"/>
+      <c r="V66" s="2"/>
+      <c r="W66" s="1">
+        <f>S66/SQRT(T65)</f>
+        <v>0.14980217325984724</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="R67" s="2"/>
+      <c r="S67" s="2"/>
+      <c r="T67" s="2"/>
+      <c r="U67" s="2"/>
+      <c r="V67" s="2"/>
+    </row>
+    <row r="68" spans="1:28">
+      <c r="A68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" t="s">
+        <v>9</v>
+      </c>
+      <c r="H68" t="s">
+        <v>11</v>
+      </c>
+      <c r="J68" t="s">
+        <v>10</v>
+      </c>
+      <c r="R68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="V68" s="2"/>
+      <c r="W68" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28">
+      <c r="A69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="3">
+        <v>3.4812899999999997E-4</v>
+      </c>
+      <c r="C69" s="8">
+        <v>5.9500000000000002E-7</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="1">
+        <f>B69^2/C65 + C69^2*0.25*B65^2/(C65)^3</f>
+        <v>2.4096263786159637E-5</v>
+      </c>
+      <c r="H69">
+        <f>F69/(D65)^2 + F70*((1-D65)/D65)^2</f>
+        <v>2.6585661973587867E-5</v>
+      </c>
+      <c r="J69">
+        <f>SQRT(H69)</f>
+        <v>5.1561285838880961E-3</v>
+      </c>
+      <c r="R69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S69" s="3">
+        <v>3.1272100000000002E-4</v>
+      </c>
+      <c r="T69" s="12">
+        <v>5.3852999999999999E-7</v>
+      </c>
+      <c r="U69" s="2"/>
+      <c r="V69" s="2"/>
+      <c r="W69" s="1">
+        <f>S69^2/T65 + T69^2*0.25*S65^2/(T65)^3</f>
+        <v>1.94439017607513E-5</v>
+      </c>
+      <c r="Y69">
+        <f>W69/(U65)^2 + W70*((1-U65)/U65)^2</f>
+        <v>2.1454885017065582E-5</v>
+      </c>
+      <c r="AA69">
+        <f>SQRT(Y69)</f>
+        <v>4.6319418192660392E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28">
+      <c r="A70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="3">
+        <v>7.3823499999999995E-4</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="1">
+        <f>B70^2/C65 + C69^2*0.25*B66^2/(C65)^3</f>
+        <v>1.0835722293097601E-4</v>
+      </c>
+      <c r="R70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S70" s="3">
+        <v>6.6714400000000005E-4</v>
+      </c>
+      <c r="T70" s="12"/>
+      <c r="U70" s="2"/>
+      <c r="V70" s="2"/>
+      <c r="W70" s="1">
+        <f>S70^2/T65 + T69^2*0.25*S66^2/(T65)^3</f>
+        <v>8.849276484886948E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2"/>
+      <c r="V71" s="2"/>
+    </row>
+    <row r="72" spans="1:28">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72">
+        <f>SQRT(F69)</f>
+        <v>4.9087945349301021E-3</v>
+      </c>
+      <c r="R72" s="2"/>
+      <c r="S72" s="2"/>
+      <c r="T72" s="2"/>
+      <c r="U72" s="2"/>
+      <c r="V72" s="2"/>
+      <c r="W72">
+        <f>SQRT(W69)</f>
+        <v>4.409523983464802E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73">
+        <f>SQRT(F70)</f>
+        <v>1.0409477553219278E-2</v>
+      </c>
+      <c r="R73" s="2"/>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
+      <c r="U73" s="2"/>
+      <c r="V73" s="2"/>
+      <c r="W73">
+        <f>SQRT(W70)</f>
+        <v>9.4070593093096566E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="R75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28">
+      <c r="A76" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" t="s">
+        <v>7</v>
+      </c>
+      <c r="K76" t="s">
+        <v>12</v>
+      </c>
+      <c r="R76" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S76" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V76" s="2"/>
+      <c r="W76" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28">
+      <c r="A77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1.0930499999999999E-2</v>
+      </c>
+      <c r="C77" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.95709599999999995</v>
+      </c>
+      <c r="E77" s="2"/>
+      <c r="F77" s="1">
+        <f>B77/SQRT(C77)</f>
+        <v>0.15412538284591909</v>
+      </c>
+      <c r="H77">
+        <f>(F77-(1-D77)*F78)/(D77)</f>
+        <v>0.15317188056321915</v>
+      </c>
+      <c r="K77">
+        <f>J81/H77</f>
+        <v>3.1950323864362098E-2</v>
+      </c>
+      <c r="R77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S77" s="3">
+        <v>1.12055E-2</v>
+      </c>
+      <c r="T77" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="U77" s="2">
+        <v>0.95709599999999995</v>
+      </c>
+      <c r="V77" s="2"/>
+      <c r="W77" s="1">
+        <f>S77/SQRT(T77)</f>
+        <v>0.15800301701477029</v>
+      </c>
+      <c r="Y77">
+        <f>(W77-(1-U77)*W78)/(U77)</f>
+        <v>0.15777116773582145</v>
+      </c>
+      <c r="AB77">
+        <f>AA81/Y77</f>
+        <v>2.7911136751951948E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28">
+      <c r="A78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1.2439E-2</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="1">
+        <f>B78/SQRT(C77)</f>
+        <v>0.17539596882305364</v>
+      </c>
+      <c r="R78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S78" s="3">
+        <v>1.1572300000000001E-2</v>
+      </c>
+      <c r="T78" s="2"/>
+      <c r="U78" s="2"/>
+      <c r="V78" s="2"/>
+      <c r="W78" s="1">
+        <f>S78/SQRT(T77)</f>
+        <v>0.16317507597162342</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="R79" s="2"/>
+      <c r="S79" s="2"/>
+      <c r="T79" s="2"/>
+      <c r="U79" s="2"/>
+      <c r="V79" s="2"/>
+    </row>
+    <row r="80" spans="1:28">
+      <c r="A80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" t="s">
+        <v>11</v>
+      </c>
+      <c r="J80" t="s">
+        <v>10</v>
+      </c>
+      <c r="R80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S80" s="2"/>
+      <c r="T80" s="2"/>
+      <c r="U80" s="2"/>
+      <c r="V80" s="2"/>
+      <c r="W80" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28">
+      <c r="A81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="3">
+        <v>3.3058399999999998E-4</v>
+      </c>
+      <c r="C81" s="8">
+        <v>5.9500000000000002E-7</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="1">
+        <f>B81^2/C77 + C81^2*0.25*B77^2/(C77)^3</f>
+        <v>2.1728692866947019E-5</v>
+      </c>
+      <c r="H81">
+        <f>F81/(D77)^2 + F82*((1-D77)/D77)^2</f>
+        <v>2.3950170988449283E-5</v>
+      </c>
+      <c r="J81">
+        <f>SQRT(H81)</f>
+        <v>4.8938911909082415E-3</v>
+      </c>
+      <c r="R81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S81" s="3">
+        <v>2.9747699999999998E-4</v>
+      </c>
+      <c r="T81" s="12">
+        <v>5.3852999999999999E-7</v>
+      </c>
+      <c r="U81" s="2"/>
+      <c r="V81" s="2"/>
+      <c r="W81" s="1">
+        <f>S81^2/T77 + T81^2*0.25*S77^2/(T77)^3</f>
+        <v>1.7594496043396074E-5</v>
+      </c>
+      <c r="Y81">
+        <f>W81/(U77)^2 + W82*((1-U77)/U77)^2</f>
+        <v>1.9391451979812651E-5</v>
+      </c>
+      <c r="AA81">
+        <f>SQRT(Y81)</f>
+        <v>4.4035726381896614E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28">
+      <c r="A82" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="3">
+        <v>7.5829900000000004E-4</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="1">
+        <f>B82^2/C77 + C81^2*0.25*B78^2/(C77)^3</f>
+        <v>1.1432722309916651E-4</v>
+      </c>
+      <c r="R82" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S82" s="3">
+        <v>6.7894899999999998E-4</v>
+      </c>
+      <c r="T82" s="12"/>
+      <c r="U82" s="2"/>
+      <c r="V82" s="2"/>
+      <c r="W82" s="1">
+        <f>S82^2/T77 + T81^2*0.25*S78^2/(T77)^3</f>
+        <v>9.1652211204154598E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="R83" s="2"/>
+      <c r="S83" s="2"/>
+      <c r="T83" s="2"/>
+      <c r="U83" s="2"/>
+      <c r="V83" s="2"/>
+    </row>
+    <row r="84" spans="1:28">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84">
+        <f>SQRT(F81)</f>
+        <v>4.6614046023647224E-3</v>
+      </c>
+      <c r="R84" s="2"/>
+      <c r="S84" s="2"/>
+      <c r="T84" s="2"/>
+      <c r="U84" s="2"/>
+      <c r="V84" s="2"/>
+      <c r="W84">
+        <f>SQRT(W81)</f>
+        <v>4.1945793642981745E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85">
+        <f>SQRT(F82)</f>
+        <v>1.0692390897229979E-2</v>
+      </c>
+      <c r="R85" s="2"/>
+      <c r="S85" s="2"/>
+      <c r="T85" s="2"/>
+      <c r="U85" s="2"/>
+      <c r="V85" s="2"/>
+      <c r="W85">
+        <f>SQRT(W82)</f>
+        <v>9.5735161358904385E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28">
+      <c r="A87" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="R87" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S87" s="2"/>
+      <c r="T87" s="2"/>
+      <c r="U87" s="2"/>
+      <c r="V87" s="2"/>
+      <c r="W87" s="2"/>
+      <c r="X87" s="2"/>
+      <c r="Y87" s="2"/>
+      <c r="Z87" s="2"/>
+      <c r="AA87" s="2"/>
+      <c r="AB87" s="2"/>
+    </row>
+    <row r="88" spans="1:28">
+      <c r="A88" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" t="s">
+        <v>5</v>
+      </c>
+      <c r="H88" t="s">
+        <v>7</v>
+      </c>
+      <c r="K88" t="s">
+        <v>12</v>
+      </c>
+      <c r="R88" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U88" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V88" s="2"/>
+      <c r="W88" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28">
+      <c r="A89" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1.30496E-2</v>
+      </c>
+      <c r="C89" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.95977100000000004</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" s="1">
+        <f>B89/SQRT(C89)</f>
+        <v>0.18400572672669191</v>
+      </c>
+      <c r="H89">
+        <f>(F89-(1-D89)*F90)/(D89)</f>
+        <v>0.18230534818562227</v>
+      </c>
+      <c r="K89">
+        <f>J93/H89</f>
+        <v>3.3873671906360522E-2</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S89" s="3">
+        <v>1.30192E-2</v>
+      </c>
+      <c r="T89" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="U89" s="2">
+        <v>0.95977100000000004</v>
+      </c>
+      <c r="V89" s="2"/>
+      <c r="W89" s="1">
+        <f>S89/SQRT(T89)</f>
+        <v>0.18357707189493527</v>
+      </c>
+      <c r="Y89">
+        <f>(W89-(1-U89)*W90)/(U89)</f>
+        <v>0.18178112463294421</v>
+      </c>
+      <c r="AB89">
+        <f>AA93/Y89</f>
+        <v>3.0533726440326536E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28">
+      <c r="A90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="3">
+        <v>1.5926599999999999E-2</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="1">
+        <f>B90/SQRT(C89)</f>
+        <v>0.22457283037681855</v>
+      </c>
+      <c r="R90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S90" s="3">
+        <v>1.60579E-2</v>
+      </c>
+      <c r="T90" s="2"/>
+      <c r="U90" s="2"/>
+      <c r="V90" s="2"/>
+      <c r="W90" s="1">
+        <f>S90/SQRT(T89)</f>
+        <v>0.22642422443634641</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="R91" s="2"/>
+      <c r="S91" s="2"/>
+      <c r="T91" s="2"/>
+      <c r="U91" s="2"/>
+      <c r="V91" s="2"/>
+    </row>
+    <row r="92" spans="1:28">
+      <c r="A92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" t="s">
+        <v>11</v>
+      </c>
+      <c r="J92" t="s">
+        <v>10</v>
+      </c>
+      <c r="R92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S92" s="2"/>
+      <c r="T92" s="2"/>
+      <c r="U92" s="2"/>
+      <c r="V92" s="2"/>
+      <c r="W92" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28">
+      <c r="A93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="3">
+        <v>4.1863300000000002E-4</v>
+      </c>
+      <c r="C93" s="8">
+        <v>5.9500000000000002E-7</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="1">
+        <f>B93^2/C89 + C93^2*0.25*B89^2/(C89)^3</f>
+        <v>3.4844695679368123E-5</v>
+      </c>
+      <c r="H93">
+        <f>F93/(D89)^2 + F94*((1-D89)/D89)^2</f>
+        <v>3.8134966781088404E-5</v>
+      </c>
+      <c r="J93">
+        <f>SQRT(H93)</f>
+        <v>6.1753515512145869E-3</v>
+      </c>
+      <c r="R93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S93" s="3">
+        <v>3.76263E-4</v>
+      </c>
+      <c r="T93" s="12">
+        <v>5.3852999999999999E-7</v>
+      </c>
+      <c r="U93" s="2"/>
+      <c r="V93" s="2"/>
+      <c r="W93" s="1">
+        <f>S93^2/T89 + T93^2*0.25*S89^2/(T89)^3</f>
+        <v>2.8148340612405528E-5</v>
+      </c>
+      <c r="Y93">
+        <f>W93/(U89)^2 + W94*((1-U89)/U89)^2</f>
+        <v>3.0807552167429901E-5</v>
+      </c>
+      <c r="AA93">
+        <f>SQRT(Y93)</f>
+        <v>5.5504551315572219E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28">
+      <c r="A94" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="3">
+        <v>9.3902000000000005E-4</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="1">
+        <f>B94^2/C89 + C93^2*0.25*B90^2/(C89)^3</f>
+        <v>1.7531472764645493E-4</v>
+      </c>
+      <c r="R94" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S94" s="3">
+        <v>8.4610800000000004E-4</v>
+      </c>
+      <c r="T94" s="12"/>
+      <c r="U94" s="2"/>
+      <c r="V94" s="2"/>
+      <c r="W94" s="1">
+        <f>S94^2/T89 + T93^2*0.25*S90^2/(T89)^3</f>
+        <v>1.4233782675970592E-4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="R95" s="2"/>
+      <c r="S95" s="2"/>
+      <c r="T95" s="2"/>
+      <c r="U95" s="2"/>
+      <c r="V95" s="2"/>
+    </row>
+    <row r="96" spans="1:28">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96">
+        <f>SQRT(F93)</f>
+        <v>5.9029395795118997E-3</v>
+      </c>
+      <c r="R96" s="2"/>
+      <c r="S96" s="2"/>
+      <c r="T96" s="2"/>
+      <c r="U96" s="2"/>
+      <c r="V96" s="2"/>
+      <c r="W96">
+        <f>SQRT(W93)</f>
+        <v>5.3055009765719139E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97">
+        <f>SQRT(F94)</f>
+        <v>1.3240646798644503E-2</v>
+      </c>
+      <c r="R97" s="2"/>
+      <c r="S97" s="2"/>
+      <c r="T97" s="2"/>
+      <c r="U97" s="2"/>
+      <c r="V97" s="2"/>
+      <c r="W97">
+        <f>SQRT(W94)</f>
+        <v>1.1930541763042696E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28">
+      <c r="A99" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+      <c r="R99" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S99" s="2"/>
+      <c r="T99" s="2"/>
+      <c r="U99" s="2"/>
+      <c r="V99" s="2"/>
+      <c r="W99" s="2"/>
+      <c r="X99" s="2"/>
+      <c r="Y99" s="2"/>
+      <c r="Z99" s="2"/>
+      <c r="AA99" s="2"/>
+      <c r="AB99" s="2"/>
+    </row>
+    <row r="100" spans="1:28">
+      <c r="A100" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="2"/>
+      <c r="F100" t="s">
+        <v>5</v>
+      </c>
+      <c r="H100" t="s">
+        <v>7</v>
+      </c>
+      <c r="K100" t="s">
+        <v>12</v>
+      </c>
+      <c r="R100" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S100" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U100" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V100" s="2"/>
+      <c r="W100" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y100" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28">
+      <c r="A101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1.5453E-2</v>
+      </c>
+      <c r="C101" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0.96200300000000005</v>
+      </c>
+      <c r="E101" s="2"/>
+      <c r="F101" s="1">
+        <f>B101/SQRT(C101)</f>
+        <v>0.21789483931366249</v>
+      </c>
+      <c r="H101">
+        <f>(F101-(1-D101)*F102)/(D101)</f>
+        <v>0.21771150639047904</v>
+      </c>
+      <c r="K101">
+        <f>J105/H101</f>
+        <v>4.7980277721505489E-2</v>
+      </c>
+      <c r="R101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S101" s="3">
+        <v>1.5479E-2</v>
+      </c>
+      <c r="T101" s="1">
+        <v>5.0295799999999996E-3</v>
+      </c>
+      <c r="U101" s="2">
+        <v>0.96200300000000005</v>
+      </c>
+      <c r="V101" s="2"/>
+      <c r="W101" s="1">
+        <f>S101/SQRT(T101)</f>
+        <v>0.21826145199871752</v>
+      </c>
+      <c r="Y101">
+        <f>(W101-(1-U101)*W102)/(U101)</f>
+        <v>0.21750991956496166</v>
+      </c>
+      <c r="AB101">
+        <f>AA105/Y101</f>
+        <v>4.3183281622891395E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28">
+      <c r="A102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="3">
+        <v>1.578218E-2</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="1">
+        <f>B102/SQRT(C101)</f>
+        <v>0.2225364379162168</v>
+      </c>
+      <c r="R102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S102" s="3">
+        <v>1.68284E-2</v>
+      </c>
+      <c r="T102" s="2"/>
+      <c r="U102" s="2"/>
+      <c r="V102" s="2"/>
+      <c r="W102" s="1">
+        <f>S102/SQRT(T101)</f>
+        <v>0.23728865035307306</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="R103" s="2"/>
+      <c r="S103" s="2"/>
+      <c r="T103" s="2"/>
+      <c r="U103" s="2"/>
+      <c r="V103" s="2"/>
+    </row>
+    <row r="104" spans="1:28">
+      <c r="A104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J104" t="s">
+        <v>10</v>
+      </c>
+      <c r="R104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S104" s="2"/>
+      <c r="T104" s="2"/>
+      <c r="U104" s="2"/>
+      <c r="V104" s="2"/>
+      <c r="W104" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y104" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28">
+      <c r="A105" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="3">
+        <v>7.1134799999999999E-4</v>
+      </c>
+      <c r="C105" s="8">
+        <v>5.9500000000000002E-7</v>
+      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="1">
+        <f>B105^2/C101 + C105^2*0.25*B101^2/(C101)^3</f>
+        <v>1.0060816461495736E-4</v>
+      </c>
+      <c r="H105">
+        <f>F105/(D101)^2 + F106*((1-D101)/D101)^2</f>
+        <v>1.0911596063314701E-4</v>
+      </c>
+      <c r="J105">
+        <f>SQRT(H105)</f>
+        <v>1.0445858539782501E-2</v>
+      </c>
+      <c r="R105" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S105" s="3">
+        <v>6.3964200000000005E-4</v>
+      </c>
+      <c r="T105" s="12">
+        <v>5.3852999999999999E-7</v>
+      </c>
+      <c r="U105" s="2"/>
+      <c r="V105" s="2"/>
+      <c r="W105" s="1">
+        <f>S105^2/T101 + T105^2*0.25*S101^2/(T101)^3</f>
+        <v>8.1347264560443369E-5</v>
+      </c>
+      <c r="Y105">
+        <f>W105/(U101)^2 + W106*((1-U101)/U101)^2</f>
+        <v>8.822454366575288E-5</v>
+      </c>
+      <c r="AA105">
+        <f>SQRT(Y105)</f>
+        <v>9.3927921123461936E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28">
+      <c r="A106" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="3">
+        <v>1.14018E-3</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="1">
+        <f>B106^2/C101 + C105^2*0.25*B102^2/(C101)^3</f>
+        <v>2.5847313371176774E-4</v>
+      </c>
+      <c r="R106" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S106" s="3">
+        <v>1.0225E-3</v>
+      </c>
+      <c r="T106" s="12"/>
+      <c r="U106" s="2"/>
+      <c r="V106" s="2"/>
+      <c r="W106" s="1">
+        <f>S106^2/T101 + T105^2*0.25*S102^2/(T101)^3</f>
+        <v>2.0787164369087032E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="R107" s="2"/>
+      <c r="S107" s="2"/>
+      <c r="T107" s="2"/>
+      <c r="U107" s="2"/>
+      <c r="V107" s="2"/>
+    </row>
+    <row r="108" spans="1:28">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108">
+        <f>SQRT(F105)</f>
+        <v>1.0030362137777348E-2</v>
+      </c>
+      <c r="R108" s="2"/>
+      <c r="S108" s="2"/>
+      <c r="T108" s="2"/>
+      <c r="U108" s="2"/>
+      <c r="V108" s="2"/>
+      <c r="W108">
+        <f>SQRT(W105)</f>
+        <v>9.0192718420304512E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109">
+        <f>SQRT(F106)</f>
+        <v>1.6077099667283514E-2</v>
+      </c>
+      <c r="R109" s="2"/>
+      <c r="S109" s="2"/>
+      <c r="T109" s="2"/>
+      <c r="U109" s="2"/>
+      <c r="V109" s="2"/>
+      <c r="W109">
+        <f>SQRT(W106)</f>
+        <v>1.4417754460763656E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="12">
+    <mergeCell ref="R26:AB26"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C93:C94"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>